<commit_message>
Kijken of het welk lukt op de laptop
</commit_message>
<xml_diff>
--- a/Results/All vs healthy.xlsx
+++ b/Results/All vs healthy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/406aaf9c23ac983a/Documenten/Thesis/Test/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="13_ncr:1_{C0FBB4DE-4BD8-4401-A523-B93CA156D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9994AE88-FD17-4FB4-83C2-BDECFEEDBF8F}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{C0FBB4DE-4BD8-4401-A523-B93CA156D99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3165798-553A-4A1C-B937-891FC7B367C9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7E266EB4-F3CB-47A9-A6C5-E89E8219E7DA}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="28800" windowHeight="15345" xr2:uid="{7E266EB4-F3CB-47A9-A6C5-E89E8219E7DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -794,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB534E20-7A20-4F67-9434-43B8E155F083}">
   <dimension ref="A1:CT52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L55" sqref="L55"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48:I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -806,7 +806,7 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
+    <col min="7" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.140625" customWidth="1"/>
     <col min="14" max="14" width="14.7109375" bestFit="1" customWidth="1"/>
@@ -3266,6 +3266,78 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AB7:AC14">
+    <cfRule type="colorScale" priority="120">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB14:AC14">
+    <cfRule type="colorScale" priority="115">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB13:AC13">
+    <cfRule type="colorScale" priority="114">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB12:AC12">
+    <cfRule type="colorScale" priority="113">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB11:AC11">
+    <cfRule type="colorScale" priority="112">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB10:AC10">
+    <cfRule type="colorScale" priority="111">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB9:AC9">
     <cfRule type="colorScale" priority="110">
       <colorScale>
         <cfvo type="min"/>
@@ -3277,80 +3349,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AB14:AC14">
-    <cfRule type="colorScale" priority="105">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB13:AC13">
-    <cfRule type="colorScale" priority="104">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB12:AC12">
-    <cfRule type="colorScale" priority="103">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB11:AC11">
-    <cfRule type="colorScale" priority="102">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB10:AC10">
-    <cfRule type="colorScale" priority="101">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB9:AC9">
-    <cfRule type="colorScale" priority="100">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AB8:AC8">
-    <cfRule type="colorScale" priority="99">
+    <cfRule type="colorScale" priority="109">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3362,7 +3362,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB7:AC7">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="108">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3374,7 +3374,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q40">
-    <cfRule type="colorScale" priority="111">
+    <cfRule type="colorScale" priority="121">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3386,7 +3386,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q41">
-    <cfRule type="colorScale" priority="113">
+    <cfRule type="colorScale" priority="123">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3398,7 +3398,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q38">
-    <cfRule type="colorScale" priority="115">
+    <cfRule type="colorScale" priority="125">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3410,7 +3410,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q39">
-    <cfRule type="colorScale" priority="117">
+    <cfRule type="colorScale" priority="127">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3422,7 +3422,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="colorScale" priority="119">
+    <cfRule type="colorScale" priority="129">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3434,7 +3434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q35">
-    <cfRule type="colorScale" priority="121">
+    <cfRule type="colorScale" priority="131">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3446,7 +3446,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q36">
-    <cfRule type="colorScale" priority="123">
+    <cfRule type="colorScale" priority="133">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3458,7 +3458,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q37">
-    <cfRule type="colorScale" priority="125">
+    <cfRule type="colorScale" priority="135">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3470,7 +3470,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q34">
-    <cfRule type="colorScale" priority="127">
+    <cfRule type="colorScale" priority="137">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3482,7 +3482,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P41:Q41">
-    <cfRule type="colorScale" priority="130">
+    <cfRule type="colorScale" priority="140">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3494,7 +3494,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40:Q40">
-    <cfRule type="colorScale" priority="133">
+    <cfRule type="colorScale" priority="143">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3506,7 +3506,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P39:Q39">
-    <cfRule type="colorScale" priority="136">
+    <cfRule type="colorScale" priority="146">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3518,7 +3518,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P38:Q38">
-    <cfRule type="colorScale" priority="139">
+    <cfRule type="colorScale" priority="149">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3530,7 +3530,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:Q37">
-    <cfRule type="colorScale" priority="142">
+    <cfRule type="colorScale" priority="152">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3542,7 +3542,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36:Q36">
-    <cfRule type="colorScale" priority="145">
+    <cfRule type="colorScale" priority="155">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3554,7 +3554,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:Q35">
-    <cfRule type="colorScale" priority="148">
+    <cfRule type="colorScale" priority="158">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3566,7 +3566,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:Q34">
-    <cfRule type="colorScale" priority="151">
+    <cfRule type="colorScale" priority="161">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3578,7 +3578,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:R34">
-    <cfRule type="colorScale" priority="154">
+    <cfRule type="colorScale" priority="164">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3590,7 +3590,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:R35">
-    <cfRule type="colorScale" priority="156">
+    <cfRule type="colorScale" priority="166">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3602,7 +3602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36:R36">
-    <cfRule type="colorScale" priority="158">
+    <cfRule type="colorScale" priority="168">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3614,7 +3614,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:R37">
-    <cfRule type="colorScale" priority="160">
+    <cfRule type="colorScale" priority="170">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3626,7 +3626,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P38:R38">
-    <cfRule type="colorScale" priority="162">
+    <cfRule type="colorScale" priority="172">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3638,7 +3638,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P39:R39">
-    <cfRule type="colorScale" priority="164">
+    <cfRule type="colorScale" priority="174">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3650,7 +3650,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40:R40">
-    <cfRule type="colorScale" priority="166">
+    <cfRule type="colorScale" priority="176">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3662,7 +3662,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P41:R41">
-    <cfRule type="colorScale" priority="168">
+    <cfRule type="colorScale" priority="178">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3674,7 +3674,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:S34">
-    <cfRule type="colorScale" priority="170">
+    <cfRule type="colorScale" priority="180">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3686,7 +3686,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:S35">
-    <cfRule type="colorScale" priority="172">
+    <cfRule type="colorScale" priority="182">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3698,7 +3698,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36:S36">
-    <cfRule type="colorScale" priority="174">
+    <cfRule type="colorScale" priority="184">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3710,7 +3710,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:S37">
-    <cfRule type="colorScale" priority="176">
+    <cfRule type="colorScale" priority="186">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3722,7 +3722,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P38:S38">
-    <cfRule type="colorScale" priority="178">
+    <cfRule type="colorScale" priority="188">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3734,7 +3734,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P39:S39">
-    <cfRule type="colorScale" priority="180">
+    <cfRule type="colorScale" priority="190">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3746,7 +3746,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P40:S40">
-    <cfRule type="colorScale" priority="182">
+    <cfRule type="colorScale" priority="192">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3758,7 +3758,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P41:S41">
-    <cfRule type="colorScale" priority="184">
+    <cfRule type="colorScale" priority="194">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3770,7 +3770,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P34:S34">
-    <cfRule type="colorScale" priority="68">
+    <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3782,7 +3782,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P35:S35">
-    <cfRule type="colorScale" priority="67">
+    <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3794,7 +3794,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P36:S36">
-    <cfRule type="colorScale" priority="66">
+    <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3806,6 +3806,90 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P37:S37">
+    <cfRule type="colorScale" priority="75">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P38:S38">
+    <cfRule type="colorScale" priority="74">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P39:S39">
+    <cfRule type="colorScale" priority="73">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P40:S40">
+    <cfRule type="colorScale" priority="72">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P41:S41">
+    <cfRule type="colorScale" priority="71">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI12:AJ12 N22">
+    <cfRule type="colorScale" priority="198">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AI13:AJ13">
+    <cfRule type="colorScale" priority="201">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AH12:AJ12 N22">
     <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
@@ -3817,7 +3901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P38:S38">
+  <conditionalFormatting sqref="AH13:AJ13">
     <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
@@ -3829,19 +3913,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P39:S39">
-    <cfRule type="colorScale" priority="63">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P40:S40">
+  <conditionalFormatting sqref="AF14:AJ14">
     <cfRule type="colorScale" priority="62">
       <colorScale>
         <cfvo type="min"/>
@@ -3853,7 +3925,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P41:S41">
+  <conditionalFormatting sqref="AF13:AJ13">
     <cfRule type="colorScale" priority="61">
       <colorScale>
         <cfvo type="min"/>
@@ -3865,80 +3937,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AI12:AJ12 N22">
-    <cfRule type="colorScale" priority="188">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AI13:AJ13">
-    <cfRule type="colorScale" priority="191">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH12:AJ12 N22">
-    <cfRule type="colorScale" priority="55">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AH13:AJ13">
-    <cfRule type="colorScale" priority="54">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF14:AJ14">
-    <cfRule type="colorScale" priority="52">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AF13:AJ13">
-    <cfRule type="colorScale" priority="51">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="AF12:AJ12">
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3950,7 +3950,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF11:AJ11">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3962,7 +3962,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI14:AJ14">
-    <cfRule type="colorScale" priority="192">
+    <cfRule type="colorScale" priority="202">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3974,7 +3974,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AI11:AJ11">
-    <cfRule type="colorScale" priority="193">
+    <cfRule type="colorScale" priority="203">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3986,7 +3986,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH11:AJ11">
-    <cfRule type="colorScale" priority="196">
+    <cfRule type="colorScale" priority="206">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3998,55 +3998,55 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH14:AJ14">
-    <cfRule type="colorScale" priority="199">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12 D12">
-    <cfRule type="colorScale" priority="229">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13 D13">
-    <cfRule type="colorScale" priority="232">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D14 K14">
-    <cfRule type="colorScale" priority="235">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D15 K15">
-    <cfRule type="colorScale" priority="238">
+    <cfRule type="colorScale" priority="209">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D12 K12">
+    <cfRule type="colorScale" priority="239">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13 K13">
+    <cfRule type="colorScale" priority="242">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K14 D14">
+    <cfRule type="colorScale" priority="245">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K15 D15">
+    <cfRule type="colorScale" priority="248">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4058,7 +4058,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF11:AJ14">
-    <cfRule type="colorScale" priority="284">
+    <cfRule type="colorScale" priority="294">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4070,7 +4070,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF11:AJ11 K12">
-    <cfRule type="colorScale" priority="286">
+    <cfRule type="colorScale" priority="296">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4082,7 +4082,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF12:AJ12 K13">
-    <cfRule type="colorScale" priority="289">
+    <cfRule type="colorScale" priority="299">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4094,7 +4094,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF13:AJ13 K14">
-    <cfRule type="colorScale" priority="292">
+    <cfRule type="colorScale" priority="302">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4106,7 +4106,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF14:AJ14 K15">
-    <cfRule type="colorScale" priority="295">
+    <cfRule type="colorScale" priority="305">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4118,7 +4118,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12">
-    <cfRule type="colorScale" priority="300">
+    <cfRule type="colorScale" priority="310">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4130,7 +4130,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K13">
-    <cfRule type="colorScale" priority="302">
+    <cfRule type="colorScale" priority="312">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4142,7 +4142,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="colorScale" priority="313">
+    <cfRule type="colorScale" priority="323">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4154,7 +4154,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15">
-    <cfRule type="colorScale" priority="315">
+    <cfRule type="colorScale" priority="325">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4166,7 +4166,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C7:I7 K7">
-    <cfRule type="colorScale" priority="321">
+    <cfRule type="colorScale" priority="331">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4178,7 +4178,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C8:I8 K8">
-    <cfRule type="colorScale" priority="324">
+    <cfRule type="colorScale" priority="334">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4190,7 +4190,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9:I9 K9">
-    <cfRule type="colorScale" priority="327">
+    <cfRule type="colorScale" priority="337">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4202,7 +4202,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11:I11 K11">
-    <cfRule type="colorScale" priority="333">
+    <cfRule type="colorScale" priority="343">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4214,7 +4214,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12:I12 K12">
-    <cfRule type="colorScale" priority="336">
+    <cfRule type="colorScale" priority="346">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4226,7 +4226,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13:I13 K13">
-    <cfRule type="colorScale" priority="339">
+    <cfRule type="colorScale" priority="349">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4238,7 +4238,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:I14 K14">
-    <cfRule type="colorScale" priority="342">
+    <cfRule type="colorScale" priority="352">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4250,7 +4250,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15:I15 K15">
-    <cfRule type="colorScale" priority="345">
+    <cfRule type="colorScale" priority="355">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4262,7 +4262,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10:I10 K10">
-    <cfRule type="colorScale" priority="357">
+    <cfRule type="colorScale" priority="367">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4274,6 +4274,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:K24">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B25:K25">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:K26">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:K27">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B28:K28">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:K29">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B30:K30">
+    <cfRule type="colorScale" priority="23">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B31:K31">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:K32">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B33:K33">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B15:K15">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -4285,7 +4405,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B25:K25">
+  <conditionalFormatting sqref="B14:K14">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
@@ -4297,7 +4417,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B26:K26">
+  <conditionalFormatting sqref="B13:K13">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -4309,7 +4429,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:K27">
+  <conditionalFormatting sqref="B12:K12">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -4321,7 +4441,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:K28">
+  <conditionalFormatting sqref="B11:K11">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
@@ -4333,7 +4453,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:K29">
+  <conditionalFormatting sqref="B10:K10">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4345,7 +4465,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B30:K30">
+  <conditionalFormatting sqref="B9:K9">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -4357,7 +4477,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:K31">
+  <conditionalFormatting sqref="B8:K8">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -4369,7 +4489,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B32:K32">
+  <conditionalFormatting sqref="B7:K7">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4381,7 +4501,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B33:K33">
+  <conditionalFormatting sqref="B43:K43">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -4393,7 +4513,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:K15">
+  <conditionalFormatting sqref="B44:K44">
     <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
@@ -4405,7 +4525,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B14:K14">
+  <conditionalFormatting sqref="B45:K45">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
@@ -4417,7 +4537,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:K13">
+  <conditionalFormatting sqref="B46:K46">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4429,7 +4549,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:K12">
+  <conditionalFormatting sqref="B47:K47">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4441,7 +4561,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:K11">
+  <conditionalFormatting sqref="B48:K48">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4453,7 +4573,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:K10">
+  <conditionalFormatting sqref="B49:K49">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4465,7 +4585,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B9:K9">
+  <conditionalFormatting sqref="B50:K50">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4477,7 +4597,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:K8">
+  <conditionalFormatting sqref="B51:K51">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4489,7 +4609,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:K7">
+  <conditionalFormatting sqref="B52:K52">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>